<commit_message>
Various changes, fixes and so on. Classes and skills are in place.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Core Imports/game_classes.xlsx
+++ b/resources/data-imports/Core Imports/game_classes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>Merchant</t>
+  </si>
+  <si>
+    <t>Dancer</t>
+  </si>
+  <si>
+    <t>Cleric</t>
+  </si>
+  <si>
+    <t>Gunslinger</t>
+  </si>
+  <si>
+    <t>Book Binder</t>
   </si>
 </sst>
 </file>
@@ -153,15 +165,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +477,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,25 +485,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="30" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="34" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="36" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="30.564" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="32.992" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="34.135" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="36.42" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -977,6 +993,128 @@
       </c>
       <c r="S12">
         <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14">
+        <v>0.15</v>
+      </c>
+      <c r="M14">
+        <v>0.03</v>
+      </c>
+      <c r="P14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>26</v>
+      </c>
+      <c r="R14">
+        <v>25</v>
+      </c>
+      <c r="S14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>0.12</v>
+      </c>
+      <c r="M15">
+        <v>0.08</v>
+      </c>
+      <c r="O15">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16">
+        <v>0.15</v>
+      </c>
+      <c r="P16" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16">
+        <v>30</v>
+      </c>
+      <c r="S16">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>